<commit_message>
ItemData 구조 바꿈, ItemDescription 추가
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/Item.xlsx
+++ b/bin/Assets/Resources/IngameData/Item.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8D38D1-95D1-4407-953B-6FCD43ECA4DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0222D951-9DC8-4DAD-8C17-0D789D6AE386}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>더미</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>날카로워 보이는 칼이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemInfoWindow에 뜰 string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날이 잘 든 단검이다
+가벼워서 쉽게 휘두를 수 있을 것 같다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>더미이다
+ㅁㄴㅇㄹ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemDescription</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -499,7 +517,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -508,17 +526,17 @@
     <col min="2" max="2" width="12.625" style="5" customWidth="1"/>
     <col min="3" max="3" width="29.375" style="5" customWidth="1"/>
     <col min="4" max="4" width="33.25" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.625" customWidth="1"/>
+    <col min="5" max="5" width="35.5" customWidth="1"/>
     <col min="6" max="6" width="30.375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -531,8 +549,11 @@
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -545,8 +566,11 @@
       <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="E3" s="9" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -559,8 +583,11 @@
       <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="E4" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -570,11 +597,11 @@
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -586,6 +613,9 @@
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>